<commit_message>
shareskill and manage listings
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidhya\Downloads\MarsFramework\MarsFramework\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neeraja_competition\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA428059-39C0-4B90-8BCF-7E49202B9138}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2C9535-2C43-47EE-9827-EAD197A87992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
     <sheet name="SignIn" sheetId="1" r:id="rId2"/>
     <sheet name="Profile" sheetId="2" r:id="rId3"/>
+    <sheet name="EditShareSkill" sheetId="5" r:id="rId4"/>
+    <sheet name="ManageListings" sheetId="6" r:id="rId5"/>
+    <sheet name="ShareSkill" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>Url</t>
   </si>
@@ -33,9 +36,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>http://www.skillswap.pro/Home</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -93,18 +93,6 @@
     <t>ConfirmPswd</t>
   </si>
   <si>
-    <t>Venugan</t>
-  </si>
-  <si>
-    <t>Vidhya</t>
-  </si>
-  <si>
-    <t>vidhyav9@gmail.com</t>
-  </si>
-  <si>
-    <t>Ithika2015</t>
-  </si>
-  <si>
     <t>Australia</t>
   </si>
   <si>
@@ -118,6 +106,117 @@
   </si>
   <si>
     <t>3 years as Oracle Developer and 2 years as Project Management Operations Lead</t>
+  </si>
+  <si>
+    <t>neerajavijay18@gmail.com</t>
+  </si>
+  <si>
+    <t>Neeraja@123</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/</t>
+  </si>
+  <si>
+    <t>Neeraja</t>
+  </si>
+  <si>
+    <t>Vijay</t>
+  </si>
+  <si>
+    <t>SubCategory</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>ServiceType</t>
+  </si>
+  <si>
+    <t>LocationType</t>
+  </si>
+  <si>
+    <t>Startdate</t>
+  </si>
+  <si>
+    <t>Enddate</t>
+  </si>
+  <si>
+    <t>Selectday</t>
+  </si>
+  <si>
+    <t>Starttime</t>
+  </si>
+  <si>
+    <t>Endtime</t>
+  </si>
+  <si>
+    <t>SkillTrade</t>
+  </si>
+  <si>
+    <t>Skill-Exchange</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>One-off service</t>
+  </si>
+  <si>
+    <t>On-site</t>
+  </si>
+  <si>
+    <t>Thurs</t>
+  </si>
+  <si>
+    <t>Performance Testing</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Programming &amp; Tech</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>19:00:00 PM</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Deleteaction</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Would like to provide selenium training for beginners</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Would like to provide Python training for beginners</t>
   </si>
 </sst>
 </file>
@@ -170,10 +269,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -516,7 +617,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,41 +631,43 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{9B4DCF24-951B-487C-840B-4A18A142B25C}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{4CE22702-CF64-48E6-A3E4-64D43655985F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -575,7 +678,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,20 +701,20 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId3" display="Test@123" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
@@ -622,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,66 +743,350 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C4B2A3-5E3D-4B49-A093-AB61871094E7}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="3">
+        <v>44663</v>
+      </c>
+      <c r="I2" s="3">
+        <v>44724</v>
+      </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>49</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="L2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4919090A-C3B9-4DB3-BF0A-5FC5B39F3726}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219CB011-4426-446F-A057-CCD87AE07DBB}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" activeCellId="1" sqref="A2:Q2 B1:Q1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="11" width="17.140625" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="3">
+        <v>44663</v>
+      </c>
+      <c r="I2" s="3">
+        <v>44693</v>
+      </c>
+      <c r="J2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>